<commit_message>
updated exp 4 codebook
</commit_message>
<xml_diff>
--- a/experiment 4/data/processed/codebook_processed_data.xlsx
+++ b/experiment 4/data/processed/codebook_processed_data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamiecummins/git/amp-intentionality/experiment 3/data/processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamiecummins/git/amp-intentionality/experiment 4/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE195DC8-EBBE-624D-B48B-8A7096A721E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C05594E-86A8-934B-A762-0CC21B353807}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="2540" windowWidth="30260" windowHeight="17540" tabRatio="583" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15440" yWindow="2580" windowWidth="30260" windowHeight="17540" tabRatio="583" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="processed_data" sheetId="14" r:id="rId1"/>
     <sheet name="trial_level_ia_amp_positive_neg" sheetId="13" r:id="rId2"/>
-    <sheet name="trial_level_amp_obama_trump_dat" sheetId="15" r:id="rId3"/>
+    <sheet name="trial_level_ia_amp_obama_trump_" sheetId="15" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>variable</t>
   </si>
@@ -59,30 +59,12 @@
     <t>Overall IA-AMP effect in the IA-AMP using positive and negative prime stimuli</t>
   </si>
   <si>
-    <t>influence_rate</t>
-  </si>
-  <si>
-    <t>The overall proportion of influenced trials to total trials in the IA-AMP</t>
-  </si>
-  <si>
     <t>awareness</t>
   </si>
   <si>
-    <t>influence_general</t>
-  </si>
-  <si>
-    <t>Self-reported influence-awareness question</t>
-  </si>
-  <si>
     <t>Self-report of frequency that target stimuli were preceded by prime stimuli</t>
   </si>
   <si>
-    <t>intentionality</t>
-  </si>
-  <si>
-    <t>Self-reported rate of intentional responding to the primes within the task</t>
-  </si>
-  <si>
     <t>self_exclusion_1</t>
   </si>
   <si>
@@ -95,12 +77,6 @@
     <t>When participant responded "do not use my data" in self_exclusion_1, they were prompted to provide a string response for why they wished to be excluded</t>
   </si>
   <si>
-    <t>unintentionality</t>
-  </si>
-  <si>
-    <t>Self-reported rate of unintentional responding to the primes within the task</t>
-  </si>
-  <si>
     <t>complete_data</t>
   </si>
   <si>
@@ -128,18 +104,6 @@
     <t>indicating whether participants responded to include their data in analyses or not</t>
   </si>
   <si>
-    <t>AMP_effect_obama_trump</t>
-  </si>
-  <si>
-    <t>Overall AMP effect in the AMP using Obama and Trump prime stimuli</t>
-  </si>
-  <si>
-    <t>demand</t>
-  </si>
-  <si>
-    <t>indicates response to question investigating demand compliance of participants to expectations of experimenter desires</t>
-  </si>
-  <si>
     <t>politics</t>
   </si>
   <si>
@@ -150,13 +114,94 @@
   </si>
   <si>
     <t>political affliliation of participants</t>
+  </si>
+  <si>
+    <t>IA_AMP_effect_obama_trump</t>
+  </si>
+  <si>
+    <t>Overall IA-AMP effect in the IA-AMP using Obama and Trump prime stimuli</t>
+  </si>
+  <si>
+    <t>IA_AMP_effect_obama_trump_influenced</t>
+  </si>
+  <si>
+    <t>IA-AMP effect in the IA-AMP using Obama and Trump prime stimuli, calculated using only those trials registered as influenced</t>
+  </si>
+  <si>
+    <t>IA_AMP_effect_obama_trump_uninfluenced</t>
+  </si>
+  <si>
+    <t>IA-AMP effect in the IA-AMP using Obama and Trump prime stimuli, calculated using only those trials not registered as influenced</t>
+  </si>
+  <si>
+    <t>influence_rate_obama_trump</t>
+  </si>
+  <si>
+    <t>The overall proportion of influenced trials to total trials in the IA-AMP using Obama and Trump stimuli</t>
+  </si>
+  <si>
+    <t>influence_rate_positive_negative</t>
+  </si>
+  <si>
+    <t>The overall proportion of influenced trials to total trials in the IA-AMP using positive and negative prime stimuli</t>
+  </si>
+  <si>
+    <t>demand_pn</t>
+  </si>
+  <si>
+    <t>indicates response to question investigating demand compliance of participants to expectations of experimenter desires in the positive-negative IA-AMP</t>
+  </si>
+  <si>
+    <t>demand_to</t>
+  </si>
+  <si>
+    <t>indicates response to question investigating demand compliance of participants to expectations of experimenter desires in the Trump-Obama IA-AMP</t>
+  </si>
+  <si>
+    <t>influence_general_pn</t>
+  </si>
+  <si>
+    <t>Self-reported influence-awareness question for the positive-negative IA-AMP</t>
+  </si>
+  <si>
+    <t>influence_general_to</t>
+  </si>
+  <si>
+    <t>Self-reported influence-awareness question for the Trump-Obama IA-AMP</t>
+  </si>
+  <si>
+    <t>intentionality_pn</t>
+  </si>
+  <si>
+    <t>Self-reported rate of intentional responding to the primes within the positive-negative IA-AMP</t>
+  </si>
+  <si>
+    <t>Self-reported rate of intentional responding to the primes within the Trump-Obama IA-AMP</t>
+  </si>
+  <si>
+    <t>intentionality_to</t>
+  </si>
+  <si>
+    <t>unintentionality_pn</t>
+  </si>
+  <si>
+    <t>unintentionality_to</t>
+  </si>
+  <si>
+    <t>Self-reported rate of unintentional responding to the primes within the positive-negative IA-AMP</t>
+  </si>
+  <si>
+    <t>Self-reported rate of unintentional responding to the primes within the Trump-Obama IA-AMP</t>
+  </si>
+  <si>
+    <t>valence type of prime: either obama (B) or Trump (A).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,6 +241,12 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1065,7 +1116,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1112,6 +1163,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="783">
@@ -2234,10 +2289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2280,110 +2335,168 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B19" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B24" s="13" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2515,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2429,52 +2542,52 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2498,10 +2611,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EE6269-E5B6-B846-B658-D01632BA4AF8}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2528,53 +2641,62 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>55</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>32</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>